<commit_message>
some new things to launch the app
</commit_message>
<xml_diff>
--- a/bin/testdata/TestData.xlsx
+++ b/bin/testdata/TestData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="2175"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13365" windowHeight="4350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:M12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -33,13 +34,22 @@
   </si>
   <si>
     <t>Secure@60</t>
+  </si>
+  <si>
+    <t>func://sports.bbc.com/showArticleById/http%3A%2F%2Fwww.bbc.co.uk%2Fsport%2Ffootball%2F37435980</t>
+  </si>
+  <si>
+    <t>func://foursquare.com/showVenueById/4c73d002d944224bc0351029</t>
+  </si>
+  <si>
+    <t>func://news.bbc.com/showArticleById/http%3A%2F%2Fwww.bbc.co.uk%2Fnews%2Fworld-middle-east-37436152</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +65,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -64,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -72,14 +88,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -363,7 +411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -403,4 +451,38 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="105.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>